<commit_message>
init project and some basics
</commit_message>
<xml_diff>
--- a/summeries of videos.docx.xlsx
+++ b/summeries of videos.docx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yotam\Documents\GitHub\HTL-HF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F97AF579-B48E-4A90-9E37-027F41D9C94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A04BBE-D06F-472B-AB76-AB58E4D47352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{368A7968-E482-42E4-AF08-94F88DF2D4C6}"/>
   </bookViews>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACE901C-1D80-4250-BE64-DBF49C7E4CF0}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:O15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33:O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update summeries of videos.docx.xlsx
</commit_message>
<xml_diff>
--- a/summeries of videos.docx.xlsx
+++ b/summeries of videos.docx.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yotam\Documents\GitHub\HTL-HF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A04BBE-D06F-472B-AB76-AB58E4D47352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F414D57A-C9D2-4DAD-BCBC-2A7EEC760B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{368A7968-E482-42E4-AF08-94F88DF2D4C6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Node" sheetId="1" r:id="rId1"/>
+    <sheet name="React" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="72">
   <si>
     <t>title</t>
   </si>
@@ -628,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACE901C-1D80-4250-BE64-DBF49C7E4CF0}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33:O33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1388,6 +1389,62 @@
     </row>
   </sheetData>
   <mergeCells count="72">
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="J11:O11"/>
+    <mergeCell ref="J12:O12"/>
+    <mergeCell ref="J13:O13"/>
+    <mergeCell ref="J26:O26"/>
+    <mergeCell ref="J15:O15"/>
+    <mergeCell ref="J16:O16"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="J18:O18"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="J20:O20"/>
     <mergeCell ref="J33:O33"/>
     <mergeCell ref="J34:O34"/>
     <mergeCell ref="J35:O35"/>
@@ -1404,62 +1461,847 @@
     <mergeCell ref="J23:O23"/>
     <mergeCell ref="J24:O24"/>
     <mergeCell ref="J25:O25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F937F1D-38F3-4189-B585-BF42380901A3}">
+  <dimension ref="A1:O36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" ref="A4:A36" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="J15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="J18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="J19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="J21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="J22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="J23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="J24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="J25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f>A25+1</f>
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="J26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="J27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="J28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="J29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="J30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="J31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="J32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="J33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="J34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="J35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="J36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="72">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="J10:O10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="J11:O11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="J12:O12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="J13:O13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:O15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:O16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="J18:O18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="J20:O20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="J21:O21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="J22:O22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="J23:O23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="J25:O25"/>
+    <mergeCell ref="B26:F26"/>
     <mergeCell ref="J26:O26"/>
-    <mergeCell ref="J15:O15"/>
-    <mergeCell ref="J16:O16"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="J18:O18"/>
-    <mergeCell ref="J19:O19"/>
-    <mergeCell ref="J20:O20"/>
-    <mergeCell ref="J9:O9"/>
-    <mergeCell ref="J10:O10"/>
-    <mergeCell ref="J11:O11"/>
-    <mergeCell ref="J12:O12"/>
-    <mergeCell ref="J13:O13"/>
-    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="J27:O27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="J28:O28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="J29:O29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="J30:O30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="J31:O31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="J32:O32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="J33:O33"/>
     <mergeCell ref="B34:F34"/>
+    <mergeCell ref="J34:O34"/>
     <mergeCell ref="B35:F35"/>
+    <mergeCell ref="J35:O35"/>
     <mergeCell ref="B36:F36"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="J36:O36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>